<commit_message>
Agregar bibliotecas, créditos, inventario y ajustes de exportación
</commit_message>
<xml_diff>
--- a/data/CUADRO DE CARGAS -INDIVIDUAL JUAN LOZANO.xlsx
+++ b/data/CUADRO DE CARGAS -INDIVIDUAL JUAN LOZANO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmontajes4\Documents\PC-JUAN LOZANO 22032022\WESTON\JUAN LOZANO\TABLA CO2\GITHUB\mi_aplicacion_python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A18AE-203B-4EDD-9311-8A9236CFE5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF40D0AC-8959-4EEA-B644-918E9A682D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="1860" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MUEBLES" sheetId="1" r:id="rId1"/>
@@ -494,9 +494,6 @@
     <t>CAJ 2464Z</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>NEU 2168U</t>
   </si>
   <si>
@@ -630,15 +627,19 @@
   </si>
   <si>
     <t xml:space="preserve">COSTO INICIAL </t>
+  </si>
+  <si>
+    <t>WEFM-004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -764,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -802,7 +803,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA194"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1625,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17">
         <v>0.95</v>
@@ -1651,7 +1654,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18">
         <v>1.25</v>
@@ -1680,7 +1683,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19">
         <v>1.9</v>
@@ -1709,7 +1712,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B20">
         <v>2.2000000000000002</v>
@@ -1738,7 +1741,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B21">
         <v>2.5</v>
@@ -1767,7 +1770,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22">
         <v>2.85</v>
@@ -1796,7 +1799,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23">
         <v>3.15</v>
@@ -1825,7 +1828,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>3.45</v>
@@ -1854,7 +1857,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25">
         <v>3.75</v>
@@ -1883,7 +1886,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26">
         <v>0.95</v>
@@ -1912,7 +1915,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B27">
         <v>1.25</v>
@@ -1941,7 +1944,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B28">
         <v>1.9</v>
@@ -1970,7 +1973,7 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B29">
         <v>2.2000000000000002</v>
@@ -1999,7 +2002,7 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B30">
         <v>2.5</v>
@@ -2028,7 +2031,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B31">
         <v>2.85</v>
@@ -2057,7 +2060,7 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32">
         <v>3.15</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B33">
         <v>3.45</v>
@@ -2115,7 +2118,7 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B34">
         <v>3.75</v>
@@ -3204,6 +3207,15 @@
       <c r="B78">
         <v>3.2</v>
       </c>
+      <c r="N78">
+        <v>1</v>
+      </c>
+      <c r="O78">
+        <v>2</v>
+      </c>
+      <c r="P78">
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -3212,6 +3224,24 @@
       <c r="B79">
         <v>2.5</v>
       </c>
+      <c r="C79">
+        <v>0.42</v>
+      </c>
+      <c r="D79">
+        <v>1.2</v>
+      </c>
+      <c r="E79">
+        <v>1.2</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
+      <c r="O79">
+        <v>2</v>
+      </c>
+      <c r="P79">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
@@ -3220,6 +3250,15 @@
       <c r="B80">
         <v>3.75</v>
       </c>
+      <c r="C80">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D80">
+        <v>2.4</v>
+      </c>
+      <c r="E80">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
@@ -5251,18 +5290,21 @@
     </row>
     <row r="171" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B171" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D171">
-        <v>1.75</v>
+        <v>0.6</v>
       </c>
       <c r="L171">
-        <v>15</v>
+        <v>8.4</v>
       </c>
       <c r="O171">
+        <v>2</v>
+      </c>
+      <c r="S171">
         <v>2</v>
       </c>
       <c r="W171">
@@ -5271,42 +5313,90 @@
     </row>
     <row r="172" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B172" t="s">
         <v>80</v>
       </c>
+      <c r="D172">
+        <v>1.2</v>
+      </c>
+      <c r="L172">
+        <v>16.7</v>
+      </c>
+      <c r="O172">
+        <v>2</v>
+      </c>
+      <c r="S172">
+        <v>2</v>
+      </c>
+      <c r="W172">
+        <v>3</v>
+      </c>
     </row>
     <row r="173" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B173" t="s">
         <v>81</v>
       </c>
+      <c r="D173">
+        <v>1.8</v>
+      </c>
+      <c r="L173">
+        <v>20</v>
+      </c>
+      <c r="O173">
+        <v>2</v>
+      </c>
+      <c r="S173">
+        <v>2</v>
+      </c>
+      <c r="W173">
+        <v>3</v>
+      </c>
     </row>
     <row r="174" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B174" t="s">
         <v>82</v>
       </c>
+      <c r="D174">
+        <v>2.4</v>
+      </c>
+      <c r="L174">
+        <v>20</v>
+      </c>
+      <c r="O174">
+        <v>2</v>
+      </c>
+      <c r="S174">
+        <v>2</v>
+      </c>
+      <c r="W174">
+        <v>3</v>
+      </c>
     </row>
     <row r="175" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B175" t="s">
         <v>83</v>
       </c>
       <c r="D175">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="L175">
-        <v>4</v>
+        <v>8.4</v>
       </c>
       <c r="O175">
+        <v>2</v>
+      </c>
+      <c r="S175">
         <v>2</v>
       </c>
       <c r="W175">
@@ -5315,74 +5405,185 @@
     </row>
     <row r="176" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B176" t="s">
         <v>84</v>
       </c>
+      <c r="D176">
+        <v>1.2</v>
+      </c>
+      <c r="L176">
+        <v>5.4</v>
+      </c>
+      <c r="O176">
+        <v>2</v>
+      </c>
+      <c r="S176">
+        <v>2</v>
+      </c>
+      <c r="W176">
+        <v>3</v>
+      </c>
     </row>
     <row r="177" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B177" t="s">
         <v>85</v>
       </c>
+      <c r="D177">
+        <v>1.8</v>
+      </c>
+      <c r="L177">
+        <v>20</v>
+      </c>
+      <c r="O177">
+        <v>2</v>
+      </c>
+      <c r="S177">
+        <v>2</v>
+      </c>
+      <c r="W177">
+        <v>3</v>
+      </c>
     </row>
     <row r="178" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178" t="s">
         <v>86</v>
       </c>
+      <c r="D178">
+        <v>2.4</v>
+      </c>
+      <c r="L178">
+        <v>20</v>
+      </c>
+      <c r="O178">
+        <v>2</v>
+      </c>
+      <c r="S178">
+        <v>2</v>
+      </c>
+      <c r="W178">
+        <v>3</v>
+      </c>
     </row>
     <row r="179" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B179" t="s">
-        <v>83</v>
+        <v>200</v>
+      </c>
+      <c r="D179">
+        <v>0.9</v>
+      </c>
+      <c r="L179">
+        <v>8.4</v>
+      </c>
+      <c r="O179">
+        <v>2</v>
+      </c>
+      <c r="S179">
+        <v>2</v>
+      </c>
+      <c r="W179">
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B180" t="s">
         <v>87</v>
       </c>
+      <c r="D180">
+        <v>1.8</v>
+      </c>
+      <c r="L180">
+        <v>16.7</v>
+      </c>
+      <c r="O180">
+        <v>2</v>
+      </c>
+      <c r="S180">
+        <v>2</v>
+      </c>
+      <c r="W180">
+        <v>3</v>
+      </c>
     </row>
     <row r="181" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B181" t="s">
         <v>88</v>
       </c>
+      <c r="D181">
+        <v>2.7</v>
+      </c>
+      <c r="L181">
+        <v>20</v>
+      </c>
+      <c r="O181">
+        <v>2</v>
+      </c>
+      <c r="S181">
+        <v>2</v>
+      </c>
+      <c r="W181">
+        <v>3</v>
+      </c>
     </row>
     <row r="182" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B182" t="s">
         <v>89</v>
       </c>
+      <c r="D182">
+        <v>3.6</v>
+      </c>
+      <c r="L182">
+        <v>20</v>
+      </c>
+      <c r="O182">
+        <v>2</v>
+      </c>
+      <c r="S182">
+        <v>2</v>
+      </c>
+      <c r="W182">
+        <v>3</v>
+      </c>
     </row>
     <row r="183" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B183" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D183">
-        <v>1.75</v>
+        <v>0.6</v>
+      </c>
+      <c r="G183">
+        <v>1.2</v>
       </c>
       <c r="L183">
-        <v>15</v>
+        <v>8.4</v>
       </c>
       <c r="O183">
+        <v>2</v>
+      </c>
+      <c r="S183">
         <v>2</v>
       </c>
       <c r="W183">
@@ -5391,42 +5592,102 @@
     </row>
     <row r="184" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B184" t="s">
         <v>80</v>
       </c>
+      <c r="D184">
+        <v>1.2</v>
+      </c>
+      <c r="G184">
+        <v>1.2</v>
+      </c>
+      <c r="L184">
+        <v>16.7</v>
+      </c>
+      <c r="O184">
+        <v>2</v>
+      </c>
+      <c r="S184">
+        <v>2</v>
+      </c>
+      <c r="W184">
+        <v>3</v>
+      </c>
     </row>
     <row r="185" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B185" t="s">
         <v>81</v>
       </c>
+      <c r="D185">
+        <v>1.8</v>
+      </c>
+      <c r="G185">
+        <v>1.2</v>
+      </c>
+      <c r="L185">
+        <v>20</v>
+      </c>
+      <c r="O185">
+        <v>2</v>
+      </c>
+      <c r="S185">
+        <v>2</v>
+      </c>
+      <c r="W185">
+        <v>3</v>
+      </c>
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B186" t="s">
         <v>82</v>
       </c>
+      <c r="D186">
+        <v>2.4</v>
+      </c>
+      <c r="G186">
+        <v>1.2</v>
+      </c>
+      <c r="L186">
+        <v>20</v>
+      </c>
+      <c r="O186">
+        <v>2</v>
+      </c>
+      <c r="S186">
+        <v>2</v>
+      </c>
+      <c r="W186">
+        <v>3</v>
+      </c>
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B187" t="s">
         <v>83</v>
       </c>
       <c r="D187">
-        <v>2</v>
+        <v>1.2</v>
+      </c>
+      <c r="G187">
+        <v>1.2</v>
       </c>
       <c r="L187">
-        <v>4</v>
+        <v>8.4</v>
       </c>
       <c r="O187">
+        <v>2</v>
+      </c>
+      <c r="S187">
         <v>2</v>
       </c>
       <c r="W187">
@@ -5435,58 +5696,184 @@
     </row>
     <row r="188" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B188" t="s">
         <v>84</v>
       </c>
+      <c r="D188">
+        <v>1.2</v>
+      </c>
+      <c r="G188">
+        <v>1.2</v>
+      </c>
+      <c r="L188">
+        <v>5.4</v>
+      </c>
+      <c r="O188">
+        <v>2</v>
+      </c>
+      <c r="S188">
+        <v>2</v>
+      </c>
+      <c r="W188">
+        <v>3</v>
+      </c>
     </row>
     <row r="189" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B189" t="s">
         <v>85</v>
       </c>
+      <c r="D189">
+        <v>1.8</v>
+      </c>
+      <c r="G189">
+        <v>1.2</v>
+      </c>
+      <c r="L189">
+        <v>20</v>
+      </c>
+      <c r="O189">
+        <v>2</v>
+      </c>
+      <c r="S189">
+        <v>2</v>
+      </c>
+      <c r="W189">
+        <v>3</v>
+      </c>
     </row>
     <row r="190" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B190" t="s">
         <v>86</v>
       </c>
+      <c r="D190">
+        <v>2.4</v>
+      </c>
+      <c r="G190">
+        <v>1.2</v>
+      </c>
+      <c r="L190">
+        <v>20</v>
+      </c>
+      <c r="O190">
+        <v>2</v>
+      </c>
+      <c r="S190">
+        <v>2</v>
+      </c>
+      <c r="W190">
+        <v>3</v>
+      </c>
     </row>
     <row r="191" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B191" t="s">
-        <v>83</v>
+        <v>200</v>
+      </c>
+      <c r="D191">
+        <v>0.9</v>
+      </c>
+      <c r="G191">
+        <v>1.2</v>
+      </c>
+      <c r="L191">
+        <v>8.4</v>
+      </c>
+      <c r="O191">
+        <v>2</v>
+      </c>
+      <c r="S191">
+        <v>2</v>
+      </c>
+      <c r="W191">
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B192" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D192">
+        <v>1.8</v>
+      </c>
+      <c r="G192">
+        <v>1.2</v>
+      </c>
+      <c r="L192">
+        <v>16.7</v>
+      </c>
+      <c r="O192">
+        <v>2</v>
+      </c>
+      <c r="S192">
+        <v>2</v>
+      </c>
+      <c r="W192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B193" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D193">
+        <v>2.7</v>
+      </c>
+      <c r="G193">
+        <v>1.2</v>
+      </c>
+      <c r="L193">
+        <v>20</v>
+      </c>
+      <c r="O193">
+        <v>2</v>
+      </c>
+      <c r="S193">
+        <v>2</v>
+      </c>
+      <c r="W193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B194" t="s">
         <v>89</v>
+      </c>
+      <c r="D194">
+        <v>3.6</v>
+      </c>
+      <c r="G194">
+        <v>1.2</v>
+      </c>
+      <c r="L194">
+        <v>20</v>
+      </c>
+      <c r="O194">
+        <v>2</v>
+      </c>
+      <c r="S194">
+        <v>2</v>
+      </c>
+      <c r="W194">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5498,8 +5885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763AEBCE-F3FC-4824-A9CA-480A7877A8C7}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6053,7 +6440,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
-        <v>13.5</v>
+        <v>7.1</v>
       </c>
       <c r="F25" s="2">
         <v>1.4</v>
@@ -6632,12 +7019,12 @@
         <v>2</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C53" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2">
@@ -6653,12 +7040,12 @@
         <v>2</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C54" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2">
@@ -6675,7 +7062,7 @@
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2">
@@ -6692,7 +7079,7 @@
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2">
@@ -6709,7 +7096,7 @@
     </row>
     <row r="57" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2">
@@ -6726,7 +7113,7 @@
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2">
@@ -6747,7 +7134,7 @@
     </row>
     <row r="59" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C59" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2">
@@ -6768,7 +7155,7 @@
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C60" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2">
@@ -6789,7 +7176,7 @@
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C61" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2">
@@ -6810,7 +7197,7 @@
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C62" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2">
@@ -6831,7 +7218,7 @@
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C63" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2">
@@ -6852,7 +7239,7 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C64" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2">
@@ -6873,7 +7260,7 @@
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C65" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2">
@@ -6894,7 +7281,7 @@
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C66" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2">
@@ -6915,7 +7302,7 @@
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C67" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2">
@@ -6936,7 +7323,7 @@
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C68" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2">
@@ -6957,7 +7344,7 @@
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C69" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2">
@@ -6978,7 +7365,7 @@
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C70" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2">
@@ -6999,7 +7386,7 @@
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C71" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2">
@@ -7025,10 +7412,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51F0C42-37E4-42E7-B0F4-77DB7EF57009}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7038,29 +7425,30 @@
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>183</v>
-      </c>
       <c r="D1" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>12</v>
       </c>
@@ -7074,13 +7462,13 @@
         <v>20</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2">
+        <v>188</v>
+      </c>
+      <c r="F2" s="20">
         <v>2700</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>10</v>
       </c>
@@ -7094,13 +7482,13 @@
         <v>30</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="F3">
+        <v>189</v>
+      </c>
+      <c r="F3" s="20">
         <v>4250</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>8</v>
       </c>
@@ -7114,13 +7502,14 @@
         <v>50</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4">
+        <v>190</v>
+      </c>
+      <c r="F4" s="20">
         <v>6400</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>6</v>
       </c>
@@ -7134,13 +7523,13 @@
         <v>65</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5">
+        <v>191</v>
+      </c>
+      <c r="F5" s="20">
         <v>9800</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -7154,13 +7543,13 @@
         <v>85</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="F6">
+        <v>192</v>
+      </c>
+      <c r="F6" s="20">
         <v>16500</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -7174,15 +7563,15 @@
         <v>115</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="F7">
+        <v>193</v>
+      </c>
+      <c r="F7" s="20">
         <v>24700</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="5">
         <v>0.39</v>
@@ -7194,15 +7583,15 @@
         <v>150</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F8">
+        <v>194</v>
+      </c>
+      <c r="F8" s="20">
         <v>39500</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="5">
         <v>0.33</v>
@@ -7214,15 +7603,15 @@
         <v>175</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9">
+        <v>195</v>
+      </c>
+      <c r="F9" s="20">
         <v>51000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="5">
         <v>0.25900000000000001</v>
@@ -7234,15 +7623,15 @@
         <v>200</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="F10">
+        <v>196</v>
+      </c>
+      <c r="F10" s="20">
         <v>82500</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="5">
         <v>0.20699999999999999</v>
@@ -7254,13 +7643,13 @@
         <v>230</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11">
+        <v>197</v>
+      </c>
+      <c r="F11" s="20">
         <v>85000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>250</v>
       </c>
@@ -7276,8 +7665,9 @@
       <c r="E12" s="9">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>300</v>
       </c>
@@ -7293,8 +7683,9 @@
       <c r="E13" s="9">
         <v>152</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>350</v>
       </c>
@@ -7310,8 +7701,9 @@
       <c r="E14" s="9">
         <v>177</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>400</v>
       </c>
@@ -7327,8 +7719,9 @@
       <c r="E15" s="9">
         <v>203</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>500</v>
       </c>
@@ -7344,8 +7737,9 @@
       <c r="E16" s="9">
         <v>253</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>600</v>
       </c>
@@ -7361,6 +7755,7 @@
       <c r="E17" s="9">
         <v>304</v>
       </c>
+      <c r="F17" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>